<commit_message>
submit fun and excel fixes exept mous and ectens activity
</commit_message>
<xml_diff>
--- a/sampleExcels/ConferenceParticipatedFaculty.xlsx
+++ b/sampleExcels/ConferenceParticipatedFaculty.xlsx
@@ -16,36 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Program Title</t>
   </si>
   <si>
-    <t>School Name</t>
-  </si>
-  <si>
-    <t>Funded By</t>
-  </si>
-  <si>
-    <t>National / International</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
     <t>sss</t>
   </si>
   <si>
-    <t>school of xyz</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>International</t>
   </si>
   <si>
     <t>2022-23</t>
+  </si>
+  <si>
+    <t>Organizing Institute</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
@@ -388,53 +382,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
@@ -454,10 +441,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"National,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"1994-95,1995-96,1996-97,1997-98,1998-99,1999-20,2000-01,2001-02,2002-03,2003-04,2004-05,2005-06,2006-07,2007-08,2008-09,2009-10,2010-11,2011-12,2012-13,2013-14,2014-15,2015-16,2016-17,2017-18,2018-19,2019-20,2020-21,2021-22,2022-23,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>